<commit_message>
checked in 3-day case study in eval
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="18120" windowHeight="19520" tabRatio="500"/>
+    <workbookView xWindow="-41180" yWindow="660" windowWidth="33660" windowHeight="17740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>CDN1</t>
   </si>
@@ -34,6 +35,15 @@
   </si>
   <si>
     <t>GO</t>
+  </si>
+  <si>
+    <t>Day A</t>
+  </si>
+  <si>
+    <t>Day B</t>
+  </si>
+  <si>
+    <t>Day C</t>
   </si>
 </sst>
 </file>
@@ -82,8 +92,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -133,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +176,11 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -178,6 +203,11 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,11 +488,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2075909000"/>
-        <c:axId val="2078256888"/>
+        <c:axId val="605473832"/>
+        <c:axId val="605476952"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2075909000"/>
+        <c:axId val="605473832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,14 +502,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078256888"/>
+        <c:crossAx val="605476952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2078256888"/>
+        <c:axId val="605476952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,21 +532,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075909000"/>
+        <c:crossAx val="605473832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -804,11 +832,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2075136760"/>
-        <c:axId val="2075833016"/>
+        <c:axId val="626346808"/>
+        <c:axId val="626349928"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2075136760"/>
+        <c:axId val="626346808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,14 +846,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075833016"/>
+        <c:crossAx val="626349928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2075833016"/>
+        <c:axId val="626349928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,21 +876,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075136760"/>
+        <c:crossAx val="626346808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -997,11 +1023,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2088113624"/>
-        <c:axId val="2070159816"/>
+        <c:axId val="626380984"/>
+        <c:axId val="626383960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088113624"/>
+        <c:axId val="626380984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2070159816"/>
+        <c:crossAx val="626383960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1018,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2070159816"/>
+        <c:axId val="626383960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,13 +1055,499 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088113624"/>
+        <c:crossAx val="626380984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$2:$C$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$2:$C$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$2:$E$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.17</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$2:$E$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.17</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$2:$G$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.19</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$2:$G$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.19</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$K$2:$K$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.09</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$K$2:$K$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.09</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="605527864"/>
+        <c:axId val="605531000"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="605527864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605531000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="605531000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Buffering ratio (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.025"/>
+              <c:y val="0.1467545202683"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605527864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1043,6 +1555,800 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$M$2:$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>24.45</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>26.04</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$M$2:$M$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>24.45</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>26.04</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2312.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2374.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2311.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$O$2:$O$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>24.51</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.52</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.06</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$O$2:$O$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>24.51</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.52</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.06</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2188.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2329.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2275.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Q$2:$Q$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>25.49</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.28</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.29</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Q$2:$Q$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>25.49</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.28</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.29</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2141.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2450.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2331.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>14.22</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14.49</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.16</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$U$2:$U$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>14.22</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14.49</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.16</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2253.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2573.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2555.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="605579928"/>
+        <c:axId val="605583064"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="605579928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605583064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="605583064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1500.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> bitrate (kbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.025"/>
+              <c:y val="0.183791557305337"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605579928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$2:$V$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$W$2:$W$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>26.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$2:$X$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>23.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="628142328"/>
+        <c:axId val="628145304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="628142328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="628145304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="628145304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> share (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0222222222222222"/>
+              <c:y val="0.239347112860892"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="628142328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1129,6 +2435,101 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1470,7 +2871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D36" activeCellId="1" sqref="A36:B38 D36:D38"/>
     </sheetView>
   </sheetViews>
@@ -1693,6 +3094,282 @@
       </c>
       <c r="E61">
         <v>24.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1.74</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <v>2.33</v>
+      </c>
+      <c r="E2">
+        <v>0.17</v>
+      </c>
+      <c r="F2">
+        <v>2.78</v>
+      </c>
+      <c r="G2">
+        <v>0.19</v>
+      </c>
+      <c r="H2">
+        <v>2.39</v>
+      </c>
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+      <c r="J2">
+        <v>1.95</v>
+      </c>
+      <c r="K2">
+        <v>0.09</v>
+      </c>
+      <c r="L2">
+        <v>2312.2399999999998</v>
+      </c>
+      <c r="M2">
+        <v>24.45</v>
+      </c>
+      <c r="N2">
+        <v>2188.8000000000002</v>
+      </c>
+      <c r="O2">
+        <v>24.51</v>
+      </c>
+      <c r="P2">
+        <v>2141.25</v>
+      </c>
+      <c r="Q2">
+        <v>25.49</v>
+      </c>
+      <c r="R2">
+        <v>2214.4699999999998</v>
+      </c>
+      <c r="S2">
+        <v>14.35</v>
+      </c>
+      <c r="T2">
+        <v>2253.1</v>
+      </c>
+      <c r="U2">
+        <v>14.22</v>
+      </c>
+      <c r="V2">
+        <v>50.36</v>
+      </c>
+      <c r="W2">
+        <v>26.61</v>
+      </c>
+      <c r="X2">
+        <v>23.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1.6</v>
+      </c>
+      <c r="C3">
+        <v>0.15</v>
+      </c>
+      <c r="D3">
+        <v>1.68</v>
+      </c>
+      <c r="E3">
+        <v>0.16</v>
+      </c>
+      <c r="F3">
+        <v>1.43</v>
+      </c>
+      <c r="G3">
+        <v>0.15</v>
+      </c>
+      <c r="H3">
+        <v>1.57</v>
+      </c>
+      <c r="I3">
+        <v>0.09</v>
+      </c>
+      <c r="J3">
+        <v>1.45</v>
+      </c>
+      <c r="K3">
+        <v>0.08</v>
+      </c>
+      <c r="L3">
+        <v>2374</v>
+      </c>
+      <c r="M3">
+        <v>26.04</v>
+      </c>
+      <c r="N3">
+        <v>2329.5</v>
+      </c>
+      <c r="O3">
+        <v>25.52</v>
+      </c>
+      <c r="P3">
+        <v>2450.0100000000002</v>
+      </c>
+      <c r="Q3">
+        <v>25.28</v>
+      </c>
+      <c r="R3">
+        <v>2384.69</v>
+      </c>
+      <c r="S3">
+        <v>14.8</v>
+      </c>
+      <c r="T3">
+        <v>2573.7800000000002</v>
+      </c>
+      <c r="U3">
+        <v>14.49</v>
+      </c>
+      <c r="V3">
+        <v>37.35</v>
+      </c>
+      <c r="W3">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="X3">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1.67</v>
+      </c>
+      <c r="C4">
+        <v>0.12</v>
+      </c>
+      <c r="D4">
+        <v>1.71</v>
+      </c>
+      <c r="E4">
+        <v>0.13</v>
+      </c>
+      <c r="F4">
+        <v>1.77</v>
+      </c>
+      <c r="G4">
+        <v>0.13</v>
+      </c>
+      <c r="H4">
+        <v>1.72</v>
+      </c>
+      <c r="I4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J4">
+        <v>1.55</v>
+      </c>
+      <c r="K4">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>2311.46</v>
+      </c>
+      <c r="M4">
+        <v>20.02</v>
+      </c>
+      <c r="N4">
+        <v>2275.6999999999998</v>
+      </c>
+      <c r="O4">
+        <v>20.059999999999999</v>
+      </c>
+      <c r="P4">
+        <v>2331.84</v>
+      </c>
+      <c r="Q4">
+        <v>20.29</v>
+      </c>
+      <c r="R4">
+        <v>2306.1999999999998</v>
+      </c>
+      <c r="S4">
+        <v>11.62</v>
+      </c>
+      <c r="T4">
+        <v>2555.2600000000002</v>
+      </c>
+      <c r="U4">
+        <v>4.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pass on sec 3 with figures
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-41180" yWindow="660" windowWidth="33660" windowHeight="17740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ab-testing" sheetId="2" r:id="rId2"/>
+    <sheet name="predictability" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>CDN1</t>
   </si>
@@ -44,6 +45,12 @@
   </si>
   <si>
     <t>Day C</t>
+  </si>
+  <si>
+    <t>5 large sites</t>
+  </si>
+  <si>
+    <t>5 large ASNs</t>
   </si>
 </sst>
 </file>
@@ -92,8 +99,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -153,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -181,6 +196,10 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -208,6 +227,10 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,11 +511,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="605473832"/>
-        <c:axId val="605476952"/>
+        <c:axId val="564714248"/>
+        <c:axId val="564717416"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="605473832"/>
+        <c:axId val="564714248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,14 +525,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605476952"/>
+        <c:crossAx val="564717416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="605476952"/>
+        <c:axId val="564717416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -532,19 +555,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605473832"/>
+        <c:crossAx val="564714248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -832,11 +857,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="626346808"/>
-        <c:axId val="626349928"/>
+        <c:axId val="564774904"/>
+        <c:axId val="564778024"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="626346808"/>
+        <c:axId val="564774904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,14 +871,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626349928"/>
+        <c:crossAx val="564778024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="626349928"/>
+        <c:axId val="564778024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,19 +901,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626346808"/>
+        <c:crossAx val="564774904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1023,11 +1050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="626380984"/>
-        <c:axId val="626383960"/>
+        <c:axId val="564809400"/>
+        <c:axId val="564812376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="626380984"/>
+        <c:axId val="564809400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626383960"/>
+        <c:crossAx val="564812376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1044,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="626383960"/>
+        <c:axId val="564812376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,13 +1082,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="626380984"/>
+        <c:crossAx val="564809400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1102,7 +1130,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'ab-testing'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1118,7 +1146,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$4</c:f>
+                <c:f>'ab-testing'!$C$2:$C$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1136,7 +1164,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$4</c:f>
+                <c:f>'ab-testing'!$C$2:$C$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1155,7 +1183,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1172,7 +1200,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>'ab-testing'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1194,7 +1222,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'ab-testing'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1210,7 +1238,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$2:$E$4</c:f>
+                <c:f>'ab-testing'!$E$2:$E$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1228,7 +1256,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$E$2:$E$4</c:f>
+                <c:f>'ab-testing'!$E$2:$E$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1247,7 +1275,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1264,7 +1292,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>'ab-testing'!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1286,7 +1314,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'ab-testing'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1302,7 +1330,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$2:$G$4</c:f>
+                <c:f>'ab-testing'!$G$2:$G$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1320,7 +1348,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$2:$G$4</c:f>
+                <c:f>'ab-testing'!$G$2:$G$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1339,7 +1367,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1356,7 +1384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$4</c:f>
+              <c:f>'ab-testing'!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1378,7 +1406,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>'ab-testing'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1402,7 +1430,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$K$2:$K$4</c:f>
+                <c:f>'ab-testing'!$K$2:$K$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1420,7 +1448,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$K$2:$K$4</c:f>
+                <c:f>'ab-testing'!$K$2:$K$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1439,7 +1467,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1456,7 +1484,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$4</c:f>
+              <c:f>'ab-testing'!$J$2:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1482,11 +1510,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="605527864"/>
-        <c:axId val="605531000"/>
+        <c:axId val="564875736"/>
+        <c:axId val="564878872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="605527864"/>
+        <c:axId val="564875736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1523,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605531000"/>
+        <c:crossAx val="564878872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1503,7 +1531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="605531000"/>
+        <c:axId val="564878872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1541,7 +1569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605527864"/>
+        <c:crossAx val="564875736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,7 +1635,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>'ab-testing'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1623,7 +1651,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$M$2:$M$4</c:f>
+                <c:f>'ab-testing'!$M$2:$M$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1641,7 +1669,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$M$2:$M$4</c:f>
+                <c:f>'ab-testing'!$M$2:$M$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1660,7 +1688,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1677,7 +1705,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$4</c:f>
+              <c:f>'ab-testing'!$L$2:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1699,7 +1727,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>'ab-testing'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1715,7 +1743,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$O$2:$O$4</c:f>
+                <c:f>'ab-testing'!$O$2:$O$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1733,7 +1761,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$O$2:$O$4</c:f>
+                <c:f>'ab-testing'!$O$2:$O$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1752,7 +1780,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1769,7 +1797,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$4</c:f>
+              <c:f>'ab-testing'!$N$2:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1791,7 +1819,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$1</c:f>
+              <c:f>'ab-testing'!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1807,7 +1835,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$Q$2:$Q$4</c:f>
+                <c:f>'ab-testing'!$Q$2:$Q$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1825,7 +1853,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$Q$2:$Q$4</c:f>
+                <c:f>'ab-testing'!$Q$2:$Q$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1844,7 +1872,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1861,7 +1889,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$2:$P$4</c:f>
+              <c:f>'ab-testing'!$P$2:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1883,7 +1911,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$1</c:f>
+              <c:f>'ab-testing'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1907,7 +1935,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$U$2:$U$4</c:f>
+                <c:f>'ab-testing'!$U$2:$U$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1925,7 +1953,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$U$2:$U$4</c:f>
+                <c:f>'ab-testing'!$U$2:$U$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1944,7 +1972,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>'ab-testing'!$A$2:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1961,7 +1989,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$4</c:f>
+              <c:f>'ab-testing'!$T$2:$T$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1987,11 +2015,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="605579928"/>
-        <c:axId val="605583064"/>
+        <c:axId val="564927800"/>
+        <c:axId val="564930936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="605579928"/>
+        <c:axId val="564927800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +2028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605583064"/>
+        <c:crossAx val="564930936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2008,7 +2036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="605583064"/>
+        <c:axId val="564930936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1500.0"/>
@@ -2050,7 +2078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="605579928"/>
+        <c:crossAx val="564927800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2116,7 +2144,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$1</c:f>
+              <c:f>'ab-testing'!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2128,7 +2156,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2142,7 +2170,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$2:$V$3</c:f>
+              <c:f>'ab-testing'!$V$2:$V$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2161,7 +2189,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$1</c:f>
+              <c:f>'ab-testing'!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2173,7 +2201,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2187,7 +2215,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$2:$W$3</c:f>
+              <c:f>'ab-testing'!$W$2:$W$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2206,7 +2234,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$1</c:f>
+              <c:f>'ab-testing'!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2218,7 +2246,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2232,7 +2260,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$X$2:$X$3</c:f>
+              <c:f>'ab-testing'!$X$2:$X$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2255,11 +2283,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="628142328"/>
-        <c:axId val="628145304"/>
+        <c:axId val="539468648"/>
+        <c:axId val="539471624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="628142328"/>
+        <c:axId val="539468648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="628145304"/>
+        <c:crossAx val="539471624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2276,7 +2304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="628145304"/>
+        <c:axId val="539471624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +2345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="628142328"/>
+        <c:crossAx val="539468648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2327,6 +2355,348 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.043</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.067</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="601126696"/>
+        <c:axId val="594228328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="601126696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="594228328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594228328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lower bound</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="601126696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2539,6 +2909,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3112,8 +3517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3370,6 +3775,86 @@
       </c>
       <c r="U4">
         <v>4.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.08</v>
+      </c>
+      <c r="D2">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C3">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F3">
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new pass on sec 3-6
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-35080" yWindow="1420" windowWidth="33600" windowHeight="20360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
   <si>
     <t>CDN1</t>
   </si>
@@ -47,10 +47,64 @@
     <t>Day C</t>
   </si>
   <si>
-    <t>5 large sites</t>
+    <t>3 large sites</t>
   </si>
   <si>
-    <t>5 large ASNs</t>
+    <t>3 large ASNs</t>
+  </si>
+  <si>
+    <t>3 large Sites</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
+  </si>
+  <si>
+    <t>ASN1</t>
+  </si>
+  <si>
+    <t>ASN2</t>
+  </si>
+  <si>
+    <t>ASN3</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Finest AC</t>
+  </si>
+  <si>
+    <t>ASN-1</t>
+  </si>
+  <si>
+    <t>ASN-2</t>
+  </si>
+  <si>
+    <t>ASN-3</t>
+  </si>
+  <si>
+    <t>ASN-4</t>
+  </si>
+  <si>
+    <t>ASN-5</t>
+  </si>
+  <si>
+    <t>Site-A</t>
+  </si>
+  <si>
+    <t>Site-B</t>
+  </si>
+  <si>
+    <t>Site-C</t>
+  </si>
+  <si>
+    <t>Site-D</t>
+  </si>
+  <si>
+    <t>Site-E</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
@@ -99,8 +153,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -168,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -200,6 +304,31 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -231,6 +360,31 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,6 +734,1322 @@
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$G$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ASN1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ASN2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ASN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$G$33:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>669.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>537.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>624.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$G$32:$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ASN1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ASN2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ASN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$G$34:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>828.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>697.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>802.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="573104792"/>
+        <c:axId val="573252632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="573104792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="573252632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573252632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="573104792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$32:$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ASN1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ASN2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ASN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$33:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.042</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$32:$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ASN1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ASN2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ASN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$34:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.056</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.042</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="598533816"/>
+        <c:axId val="658599496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="598533816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="658599496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="658599496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="598533816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>5 Largest ASNs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$50:$F$50</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>ASN-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ASN-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ASN-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ASN-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ASN-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$51:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.042</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.037</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.028</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="595395048"/>
+        <c:axId val="576463480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="595395048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="576463480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="576463480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lower bound</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="595395048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>5 Largest Sites</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$56:$F$56</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Site-D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Site-E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$57:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.091</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.045</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.054</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="647463512"/>
+        <c:axId val="659456424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="647463512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="659456424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="659456424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lower bound</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="647463512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$41:$D$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$42:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.053</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.091</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.045</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$41:$D$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$43:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.063</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$41:$D$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$44:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="648241672"/>
+        <c:axId val="679719816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="648241672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="679719816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="679719816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Overall prediction error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="648241672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lower bound</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$G$41:$I$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$G$42:$I$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>384.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1699.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>379.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$G$41:$I$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$G$43:$I$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>519.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2268.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>511.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$G$41:$I$41</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$G$44:$I$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1420.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2460.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1280.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="658871768"/>
+        <c:axId val="658874264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="658871768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="658874264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="658874264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Overall prediction error (Kbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="658871768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2411,11 +3881,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$B$1</c:f>
+              <c:f>'ab-testing'!$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>CDN1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2423,29 +3893,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$B$2:$B$3</c:f>
+              <c:f>'ab-testing'!$B$29:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.072</c:v>
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2456,11 +3926,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$C$1</c:f>
+              <c:f>'ab-testing'!$D$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>CDN2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2468,29 +3938,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$C$2:$C$3</c:f>
+              <c:f>'ab-testing'!$D$29:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.043</c:v>
+                  <c:v>1.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2501,11 +3971,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$D$1</c:f>
+              <c:f>'ab-testing'!$F$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>CDN3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2513,29 +3983,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$D$2:$D$3</c:f>
+              <c:f>'ab-testing'!$F$29:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.044</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.035</c:v>
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2546,11 +4016,192 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$E$1</c:f>
+              <c:f>'ab-testing'!$J$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ab-testing'!$J$29:$J$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="539481336"/>
+        <c:axId val="606496584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="539481336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="606496584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="606496584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Buffering ratio (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0277777777777778"/>
+              <c:y val="0.105087853601633"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539481336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ab-testing'!$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2558,14 +4209,458 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ab-testing'!$L$29:$L$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2368.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2311.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ab-testing'!$N$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ab-testing'!$N$29:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2308.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2275.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ab-testing'!$P$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ab-testing'!$P$29:$P$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2413.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2331.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ab-testing'!$T$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ab-testing'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ab-testing'!$T$29:$T$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2589.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2555.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="642737080"/>
+        <c:axId val="652215896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="642737080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="652215896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="652215896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average bitrate (Kbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="642737080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
               <c:f>predictability!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 large ASNs</c:v>
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.043</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2607,10 +4702,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 large ASNs</c:v>
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2701,24 +4796,6 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1800">
-          <a:latin typeface="Arial"/>
-          <a:cs typeface="Arial"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2914,6 +4991,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2921,16 +5058,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2944,6 +5081,186 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3515,10 +5832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3774,6 +6091,165 @@
         <v>2555.2600000000002</v>
       </c>
       <c r="U4">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" t="s">
+        <v>3</v>
+      </c>
+      <c r="T28" t="s">
+        <v>4</v>
+      </c>
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
+        <v>1</v>
+      </c>
+      <c r="X28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1.75</v>
+      </c>
+      <c r="C29">
+        <v>0.17</v>
+      </c>
+      <c r="D29">
+        <v>1.71</v>
+      </c>
+      <c r="E29">
+        <v>0.16</v>
+      </c>
+      <c r="F29">
+        <v>1.61</v>
+      </c>
+      <c r="G29">
+        <v>0.17</v>
+      </c>
+      <c r="J29">
+        <v>1.56</v>
+      </c>
+      <c r="K29">
+        <v>0.02</v>
+      </c>
+      <c r="L29">
+        <v>2368.7800000000002</v>
+      </c>
+      <c r="M29">
+        <v>27.61</v>
+      </c>
+      <c r="N29">
+        <v>2308.5100000000002</v>
+      </c>
+      <c r="O29">
+        <v>27.67</v>
+      </c>
+      <c r="P29">
+        <v>2413.5</v>
+      </c>
+      <c r="Q29">
+        <v>27.28</v>
+      </c>
+      <c r="T29">
+        <v>2589.14</v>
+      </c>
+      <c r="U29">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>1.67</v>
+      </c>
+      <c r="C30">
+        <v>0.12</v>
+      </c>
+      <c r="D30">
+        <v>1.71</v>
+      </c>
+      <c r="E30">
+        <v>0.13</v>
+      </c>
+      <c r="F30">
+        <v>1.77</v>
+      </c>
+      <c r="G30">
+        <v>0.13</v>
+      </c>
+      <c r="H30">
+        <v>1.72</v>
+      </c>
+      <c r="I30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J30">
+        <v>1.55</v>
+      </c>
+      <c r="K30">
+        <v>0.03</v>
+      </c>
+      <c r="L30">
+        <v>2311.46</v>
+      </c>
+      <c r="M30">
+        <v>20.02</v>
+      </c>
+      <c r="N30">
+        <v>2275.6999999999998</v>
+      </c>
+      <c r="O30">
+        <v>20.059999999999999</v>
+      </c>
+      <c r="P30">
+        <v>2331.84</v>
+      </c>
+      <c r="Q30">
+        <v>20.29</v>
+      </c>
+      <c r="R30">
+        <v>2306.1999999999998</v>
+      </c>
+      <c r="S30">
+        <v>11.62</v>
+      </c>
+      <c r="T30">
+        <v>2555.2600000000002</v>
+      </c>
+      <c r="U30">
         <v>4.16</v>
       </c>
     </row>
@@ -3791,9 +6267,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3855,6 +6333,306 @@
       </c>
       <c r="F3">
         <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D26">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F26">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C33">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D33">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <v>669</v>
+      </c>
+      <c r="H33">
+        <v>537</v>
+      </c>
+      <c r="I33">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C34">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D34">
+        <v>0.09</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>828</v>
+      </c>
+      <c r="H34">
+        <v>697</v>
+      </c>
+      <c r="I34">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C42">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D42">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>384</v>
+      </c>
+      <c r="H42">
+        <v>1699</v>
+      </c>
+      <c r="I42">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C43">
+        <v>0.115</v>
+      </c>
+      <c r="D43">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>519</v>
+      </c>
+      <c r="H43">
+        <v>2268</v>
+      </c>
+      <c r="I43">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>0.12</v>
+      </c>
+      <c r="C44">
+        <v>0.18</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44">
+        <v>1420</v>
+      </c>
+      <c r="H44">
+        <v>2460</v>
+      </c>
+      <c r="I44">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C45">
+        <v>0.128</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <v>600</v>
+      </c>
+      <c r="H45">
+        <v>2410</v>
+      </c>
+      <c r="I45">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C51">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D51">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E51">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F51">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="C57">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D57">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E57">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F57">
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in sec 6
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-42320" yWindow="3340" windowWidth="33600" windowHeight="19180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-42320" yWindow="3340" windowWidth="33600" windowHeight="19180" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
     <sheet name="ab-testing" sheetId="2" r:id="rId2"/>
     <sheet name="predictability" sheetId="3" r:id="rId3"/>
+    <sheet name="improvement" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
   <si>
     <t>CDN1</t>
   </si>
@@ -106,6 +107,21 @@
   <si>
     <t>]</t>
   </si>
+  <si>
+    <t>Buffering ratio</t>
+  </si>
+  <si>
+    <t>Start failure rate</t>
+  </si>
+  <si>
+    <t>Join time (ms)</t>
+  </si>
+  <si>
+    <t>Average bitrate (Kbps)</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
 </sst>
 </file>
 
@@ -153,8 +169,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -329,6 +349,8 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -385,6 +407,8 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,11 +689,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564714248"/>
-        <c:axId val="564717416"/>
+        <c:axId val="569762264"/>
+        <c:axId val="569765384"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="564714248"/>
+        <c:axId val="569762264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,14 +703,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564717416"/>
+        <c:crossAx val="569765384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="564717416"/>
+        <c:axId val="569765384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,21 +733,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564714248"/>
+        <c:crossAx val="569762264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -870,11 +892,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="573104792"/>
-        <c:axId val="573252632"/>
+        <c:axId val="570197016"/>
+        <c:axId val="570199992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="573104792"/>
+        <c:axId val="570197016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="573252632"/>
+        <c:crossAx val="570199992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -891,7 +913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="573252632"/>
+        <c:axId val="570199992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="573104792"/>
+        <c:crossAx val="570197016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1056,11 +1078,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="598533816"/>
-        <c:axId val="658599496"/>
+        <c:axId val="570228648"/>
+        <c:axId val="570231624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="598533816"/>
+        <c:axId val="570228648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658599496"/>
+        <c:crossAx val="570231624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="658599496"/>
+        <c:axId val="570231624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="598533816"/>
+        <c:crossAx val="570228648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1210,11 +1232,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="595395048"/>
-        <c:axId val="576463480"/>
+        <c:axId val="570258152"/>
+        <c:axId val="570261096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="595395048"/>
+        <c:axId val="570258152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,7 +1245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="576463480"/>
+        <c:crossAx val="570261096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1231,7 +1253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="576463480"/>
+        <c:axId val="570261096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,7 +1283,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595395048"/>
+        <c:crossAx val="570258152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1396,11 +1418,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="647463512"/>
-        <c:axId val="659456424"/>
+        <c:axId val="570290152"/>
+        <c:axId val="570293096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="647463512"/>
+        <c:axId val="570290152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,7 +1431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="659456424"/>
+        <c:crossAx val="570293096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1417,7 +1439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="659456424"/>
+        <c:axId val="570293096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="647463512"/>
+        <c:crossAx val="570290152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1665,11 +1687,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="648241672"/>
-        <c:axId val="679719816"/>
+        <c:axId val="570330360"/>
+        <c:axId val="570333336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="648241672"/>
+        <c:axId val="570330360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1678,7 +1700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="679719816"/>
+        <c:crossAx val="570333336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1686,7 +1708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="679719816"/>
+        <c:axId val="570333336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,7 +1738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="648241672"/>
+        <c:crossAx val="570330360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1939,11 +1961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="658871768"/>
-        <c:axId val="658874264"/>
+        <c:axId val="570368088"/>
+        <c:axId val="570371064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="658871768"/>
+        <c:axId val="570368088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658874264"/>
+        <c:crossAx val="570371064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1960,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="658874264"/>
+        <c:axId val="570371064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +2012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="658871768"/>
+        <c:crossAx val="570368088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,6 +2022,661 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>improvement!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buffering ratio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>improvement!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>improvement!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.848075029357</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.74065602498121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4943380421973</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="594146744"/>
+        <c:axId val="594139880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="594146744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="594139880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594139880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="594146744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>improvement!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average bitrate (Kbps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>improvement!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>improvement!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1159.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2012.3834</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.3788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>858.1924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="594165544"/>
+        <c:axId val="593497576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="594165544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="593497576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593497576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="594165544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>improvement!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Join time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>improvement!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>improvement!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>732.3052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3391.3236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.2794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2689.6142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="142952888"/>
+        <c:axId val="143404696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="142952888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143404696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="143404696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142952888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>improvement!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start failure rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>improvement!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>improvement!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="620093960"/>
+        <c:axId val="620254664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="620093960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="620254664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="620254664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="620093960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2303,11 +2980,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564774904"/>
-        <c:axId val="564778024"/>
+        <c:axId val="569839240"/>
+        <c:axId val="569842360"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="564774904"/>
+        <c:axId val="569839240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,14 +2994,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564778024"/>
+        <c:crossAx val="569842360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="564778024"/>
+        <c:axId val="569842360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,21 +3024,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564774904"/>
+        <c:crossAx val="569839240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2496,11 +3171,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564809400"/>
-        <c:axId val="564812376"/>
+        <c:axId val="569873384"/>
+        <c:axId val="569876360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="564809400"/>
+        <c:axId val="569873384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,7 +3184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564812376"/>
+        <c:crossAx val="569876360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2517,7 +3192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="564812376"/>
+        <c:axId val="569876360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,14 +3203,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564809400"/>
+        <c:crossAx val="569873384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2956,11 +3630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564875736"/>
-        <c:axId val="564878872"/>
+        <c:axId val="569938552"/>
+        <c:axId val="569941688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="564875736"/>
+        <c:axId val="569938552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2969,7 +3643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564878872"/>
+        <c:crossAx val="569941688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2977,7 +3651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="564878872"/>
+        <c:axId val="569941688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -3015,14 +3689,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564875736"/>
+        <c:crossAx val="569938552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3461,11 +4134,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="564927800"/>
-        <c:axId val="564930936"/>
+        <c:axId val="569990936"/>
+        <c:axId val="569994072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="564927800"/>
+        <c:axId val="569990936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3474,7 +4147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564930936"/>
+        <c:crossAx val="569994072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3482,7 +4155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="564930936"/>
+        <c:axId val="569994072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1500.0"/>
@@ -3524,14 +4197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="564927800"/>
+        <c:crossAx val="569990936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3729,11 +4401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="539468648"/>
-        <c:axId val="539471624"/>
+        <c:axId val="570025448"/>
+        <c:axId val="570028424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539468648"/>
+        <c:axId val="570025448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,7 +4414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539471624"/>
+        <c:crossAx val="570028424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3750,7 +4422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539471624"/>
+        <c:axId val="570028424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3791,14 +4463,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539468648"/>
+        <c:crossAx val="570025448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4049,11 +4720,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="539481336"/>
-        <c:axId val="606496584"/>
+        <c:axId val="570068280"/>
+        <c:axId val="570071272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539481336"/>
+        <c:axId val="570068280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4062,7 +4733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="606496584"/>
+        <c:crossAx val="570071272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4070,7 +4741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="606496584"/>
+        <c:axId val="570071272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4108,14 +4779,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539481336"/>
+        <c:crossAx val="570068280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4366,11 +5036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="642737080"/>
-        <c:axId val="652215896"/>
+        <c:axId val="570109768"/>
+        <c:axId val="570112760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="642737080"/>
+        <c:axId val="570109768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4379,7 +5049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="652215896"/>
+        <c:crossAx val="570112760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4387,7 +5057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652215896"/>
+        <c:axId val="570112760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -4411,21 +5081,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="642737080"/>
+        <c:crossAx val="570109768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4713,11 +5381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="601126696"/>
-        <c:axId val="594228328"/>
+        <c:axId val="570165832"/>
+        <c:axId val="570168888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="601126696"/>
+        <c:axId val="570165832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4727,7 +5395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="594228328"/>
+        <c:crossAx val="570168888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4735,7 +5403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="594228328"/>
+        <c:axId val="570168888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4758,14 +5426,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="601126696"/>
+        <c:crossAx val="570165832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5247,6 +5914,131 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6247,7 +7039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
@@ -6611,6 +7403,113 @@
       </c>
       <c r="F57">
         <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>1.3</v>
+      </c>
+      <c r="C2">
+        <v>1159</v>
+      </c>
+      <c r="D2">
+        <v>732.30520000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>4.8480750293570001</v>
+      </c>
+      <c r="C3">
+        <v>2012.3833999999999</v>
+      </c>
+      <c r="D3">
+        <v>3391.3236000000002</v>
+      </c>
+      <c r="E3">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>2.74065602498121</v>
+      </c>
+      <c r="C4">
+        <v>160.37880000000001</v>
+      </c>
+      <c r="D4">
+        <v>500.27940000000001</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>1.4943380421973</v>
+      </c>
+      <c r="C5">
+        <v>858.19240000000002</v>
+      </c>
+      <c r="D5">
+        <v>2689.6142</v>
+      </c>
+      <c r="E5">
+        <v>4.08</v>
+      </c>
+      <c r="F5">
+        <v>9.0800000000000006E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proof reading for sec 4
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>ASN3</t>
   </si>
   <si>
-    <t>Baseline</t>
-  </si>
-  <si>
     <t>Finest AC</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   <si>
     <t>Global</t>
   </si>
+  <si>
+    <t>Strawman</t>
+  </si>
 </sst>
 </file>
 
@@ -169,8 +169,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -292,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +353,7 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -409,6 +412,7 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1636,7 +1640,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Baseline</c:v>
+                  <c:v>Strawman</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1924,7 +1928,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Baseline</c:v>
+                  <c:v>Strawman</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6638,8 +6642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7073,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="S56" sqref="S56"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7243,22 +7247,22 @@
     </row>
     <row r="41" spans="1:9">
       <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>23</v>
       </c>
-      <c r="D41" t="s">
-        <v>24</v>
-      </c>
       <c r="G41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" t="s">
         <v>22</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>23</v>
-      </c>
-      <c r="I41" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -7315,7 +7319,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B44">
         <v>1.2</v>
@@ -7327,7 +7331,7 @@
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G44">
         <v>1420</v>
@@ -7341,7 +7345,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45">
         <v>6.7000000000000004E-2</v>
@@ -7350,10 +7354,10 @@
         <v>0.128</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>600</v>
@@ -7367,19 +7371,19 @@
     </row>
     <row r="50" spans="1:6">
       <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
         <v>17</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>18</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>19</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>20</v>
-      </c>
-      <c r="F50" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -7404,19 +7408,19 @@
     </row>
     <row r="56" spans="1:6">
       <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
         <v>22</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>23</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>24</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>25</v>
-      </c>
-      <c r="F56" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -7463,21 +7467,21 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1.3</v>
@@ -7494,7 +7498,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>4.8480750293570001</v>
@@ -7511,7 +7515,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>2.74065602498121</v>
@@ -7528,7 +7532,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1.4943380421973</v>

</xml_diff>

<commit_message>
pass on sec 6
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
@@ -4780,6 +4780,7 @@
         <c:axId val="570071272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5096,6 +5097,7 @@
         <c:axId val="570112760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5678,8 +5680,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -5708,8 +5710,8 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -6642,8 +6644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7077,7 +7079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new figures for sec 4, new flow for sec 6
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-44920" yWindow="3180" windowWidth="33600" windowHeight="19060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,10 @@
     <sheet name="predictability" sheetId="3" r:id="rId3"/>
     <sheet name="improvement" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">predictability!$A$41:$D$45</definedName>
+  </definedNames>
+  <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
   <si>
     <t>CDN1</t>
   </si>
@@ -169,8 +172,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -294,7 +301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +361,8 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -413,6 +422,8 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1670,7 +1681,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.2</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>18.0</c:v>
@@ -2092,6 +2103,476 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$61:$D$61</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$63:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strawman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$61:$D$61</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$64:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="112527608"/>
+        <c:axId val="112532280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="112527608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112532280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112532280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Approx. rate to LB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0305555555555555"/>
+              <c:y val="0.174532298046078"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112527608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$70</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$68:$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$70:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$A$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Strawman</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$B$68:$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$71:$D$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="641436184"/>
+        <c:axId val="593730504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="641436184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="593730504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593730504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Approx. </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>rate</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> to LB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0277777777777778"/>
+              <c:y val="0.151384149897929"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="641436184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Aira"/>
+          <a:cs typeface="Aira"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
@@ -2251,7 +2732,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2414,7 +2895,351 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 Amazon'!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$C$12:$C$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>22.86</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.45</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$C$12:$C$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>22.86</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.45</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>41973.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1 Amazon'!$B$12:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2319.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2312.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 Amazon'!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$E$12:$E$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>22.98</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.51</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$E$12:$E$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>22.98</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>24.51</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>41973.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1 Amazon'!$D$12:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2227.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2188.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 Amazon'!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CDN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$G$12:$G$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>23.4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.49</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'1 Amazon'!$G$12:$G$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>23.4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.49</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>41973.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1 Amazon'!$F$12:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2210.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2141.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="569839240"/>
+        <c:axId val="569842360"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="569839240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="569842360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="569842360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average bitrate (Kbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="569839240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2577,7 +3402,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2732,350 +3557,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="1"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1 Amazon'!$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CDN1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$C$12:$C$14</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>22.86</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>24.45</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$C$12:$C$13</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
-                  <c:pt idx="0">
-                    <c:v>22.86</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>24.45</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>41973.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41974.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'1 Amazon'!$B$12:$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2319.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2312.24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1 Amazon'!$D$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CDN2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$E$12:$E$13</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
-                  <c:pt idx="0">
-                    <c:v>22.98</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>24.51</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$E$12:$E$13</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
-                  <c:pt idx="0">
-                    <c:v>22.98</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>24.51</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>41973.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41974.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'1 Amazon'!$D$12:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2227.57</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2188.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1 Amazon'!$F$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CDN3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$G$12:$G$13</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
-                  <c:pt idx="0">
-                    <c:v>23.4</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25.49</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'1 Amazon'!$G$12:$G$13</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
-                  <c:pt idx="0">
-                    <c:v>23.4</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25.49</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'1 Amazon'!$A$12:$A$13</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>41973.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41974.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'1 Amazon'!$F$12:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2210.15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2141.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="569839240"/>
-        <c:axId val="569842360"/>
-      </c:barChart>
-      <c:dateAx>
-        <c:axId val="569839240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569842360"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="569842360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Average bitrate (Kbps)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569839240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -5951,6 +6432,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6644,8 +7185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7077,10 +7618,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7324,7 +7865,7 @@
         <v>32</v>
       </c>
       <c r="B44">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>18</v>
@@ -7443,6 +7984,112 @@
       </c>
       <c r="F57">
         <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62">
+        <v>5.3</v>
+      </c>
+      <c r="C62">
+        <v>9.1</v>
+      </c>
+      <c r="D62">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>1.2</v>
+      </c>
+      <c r="C63">
+        <v>1.21</v>
+      </c>
+      <c r="D63">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>2.4</v>
+      </c>
+      <c r="C64">
+        <v>1.9</v>
+      </c>
+      <c r="D64">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>384</v>
+      </c>
+      <c r="C69">
+        <v>1699</v>
+      </c>
+      <c r="D69">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>1.3</v>
+      </c>
+      <c r="C70">
+        <v>1.35</v>
+      </c>
+      <c r="D70">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71">
+        <v>3.8</v>
+      </c>
+      <c r="C71">
+        <v>1.55</v>
+      </c>
+      <c r="D71">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pass on sec 5
</commit_message>
<xml_diff>
--- a/figures/ab-tesging.xlsx
+++ b/figures/ab-tesging.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-44920" yWindow="3180" windowWidth="33600" windowHeight="19060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 Amazon" sheetId="1" r:id="rId1"/>
     <sheet name="ab-testing" sheetId="2" r:id="rId2"/>
     <sheet name="predictability" sheetId="3" r:id="rId3"/>
     <sheet name="improvement" sheetId="4" r:id="rId4"/>
+    <sheet name="improvRate" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">predictability!$A$41:$D$45</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="33">
   <si>
     <t>CDN1</t>
   </si>
@@ -172,8 +173,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -301,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +368,8 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -424,6 +431,8 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -782,6 +791,330 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.043</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.032</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.067</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictability!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3 large sites</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 large ASNs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictability!$F$2:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="570165832"/>
+        <c:axId val="570168888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="570165832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="570168888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="570168888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lower bound</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="570165832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
@@ -961,7 +1294,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1147,7 +1480,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1333,7 +1666,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1519,7 +1852,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1807,7 +2140,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2096,7 +2429,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2326,7 +2659,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2566,7 +2899,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2698,169 +3031,6 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="594146744"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1800" b="0">
-          <a:latin typeface="Arial"/>
-          <a:cs typeface="Arial"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>improvement!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average bitrate (Kbps)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>improvement!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Site-A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Site-B</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Site-C</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Global</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>improvement!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1159.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2012.3834</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>160.3788</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>858.1924</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:axId val="594165544"/>
-        <c:axId val="593497576"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="594165544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="593497576"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="593497576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="594165544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3265,6 +3435,169 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>improvement!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average bitrate (Kbps)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>improvement!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Site-A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Site-B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Site-C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>improvement!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1159.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2012.3834</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.3788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>858.1924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="594165544"/>
+        <c:axId val="593497576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="594165544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="593497576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593497576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="594165544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800" b="0">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>improvement!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -3402,7 +3735,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4126,7 +4459,7 @@
                   <c:v>1.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.45</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.55</c:v>
@@ -5672,11 +6005,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$B$1</c:f>
+              <c:f>'ab-testing'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>CDN1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5684,29 +6017,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$B$2:$B$3</c:f>
+              <c:f>'ab-testing'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.072</c:v>
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5717,11 +6050,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$C$1</c:f>
+              <c:f>'ab-testing'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>CDN2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5729,29 +6062,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$C$2:$C$3</c:f>
+              <c:f>'ab-testing'!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.043</c:v>
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5762,11 +6095,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$D$1</c:f>
+              <c:f>'ab-testing'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>CDN3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5774,29 +6107,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$D$2:$D$3</c:f>
+              <c:f>'ab-testing'!$F$2:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.044</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.035</c:v>
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5807,86 +6140,49 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>predictability!$E$1</c:f>
+              <c:f>'ab-testing'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>GO</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
+              <c:f>'ab-testing'!$A$2:$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 large ASNs</c:v>
+                  <c:v>Day A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>predictability!$E$2:$E$3</c:f>
+              <c:f>'ab-testing'!$J$2:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.032</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.067</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>predictability!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>predictability!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3 large sites</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 large ASNs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>predictability!$F$2:$F$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.062</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.044</c:v>
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5901,21 +6197,20 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="570165832"/>
-        <c:axId val="570168888"/>
+        <c:axId val="632521384"/>
+        <c:axId val="620726776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570165832"/>
+        <c:axId val="632521384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570168888"/>
+        <c:crossAx val="620726776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5923,7 +6218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="570168888"/>
+        <c:axId val="620726776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5941,27 +6236,57 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Lower bound</a:t>
+                  <a:t>Buffering ratio (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0222222222222222"/>
+              <c:y val="0.123606372120152"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570165832"/>
+        <c:crossAx val="632521384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800">
+          <a:latin typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -6159,16 +6484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6189,14 +6514,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
@@ -6212,6 +6537,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7185,8 +7540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7335,7 +7690,7 @@
         <v>0.09</v>
       </c>
       <c r="J3">
-        <v>1.45</v>
+        <v>1.43</v>
       </c>
       <c r="K3">
         <v>0.08</v>
@@ -7620,7 +7975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
@@ -8109,7 +8464,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8209,4 +8564,106 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1.3</v>
+      </c>
+      <c r="C2">
+        <v>1159</v>
+      </c>
+      <c r="D2">
+        <v>732.30520000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>4.8480750293570001</v>
+      </c>
+      <c r="C3">
+        <v>2012.3833999999999</v>
+      </c>
+      <c r="D3">
+        <v>3391.3236000000002</v>
+      </c>
+      <c r="E3">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>2.74065602498121</v>
+      </c>
+      <c r="C4">
+        <v>160.37880000000001</v>
+      </c>
+      <c r="D4">
+        <v>500.27940000000001</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1.4943380421973</v>
+      </c>
+      <c r="C5">
+        <v>858.19240000000002</v>
+      </c>
+      <c r="D5">
+        <v>2689.6142</v>
+      </c>
+      <c r="E5">
+        <v>4.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>